<commit_message>
main work is done; corr. calculated
</commit_message>
<xml_diff>
--- a/src/Kriminalita.xlsx
+++ b/src/Kriminalita.xlsx
@@ -7,16 +7,17 @@
     <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="13995"/>
   </bookViews>
   <sheets>
-    <sheet name="DATA" sheetId="1" r:id="rId1"/>
-    <sheet name="UKAZATELE" sheetId="2" r:id="rId2"/>
-    <sheet name="METAINFORMACE" sheetId="3" r:id="rId3"/>
+    <sheet name="src" sheetId="4" r:id="rId1"/>
+    <sheet name="DATA" sheetId="1" r:id="rId2"/>
+    <sheet name="UKAZATELE" sheetId="2" r:id="rId3"/>
+    <sheet name="METAINFORMACE" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="245">
   <si>
     <t>Data z Veřejné databáze ČSU</t>
   </si>
@@ -750,6 +751,15 @@
   </si>
   <si>
     <t>Český statistický úřad, Veřejná databáze</t>
+  </si>
+  <si>
+    <t>okres</t>
+  </si>
+  <si>
+    <t>kriminalita</t>
+  </si>
+  <si>
+    <t>vloupani</t>
   </si>
 </sst>
 </file>
@@ -1307,9 +1317,1955 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C246"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>242</v>
+      </c>
+      <c r="B1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C1" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="str">
+        <f>DATA!B8</f>
+        <v>Hlavní město Praha</v>
+      </c>
+      <c r="B2">
+        <f>DATA!C8</f>
+        <v>64095</v>
+      </c>
+      <c r="C2">
+        <f>DATA!G8</f>
+        <v>1761</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="18" t="str">
+        <f>DATA!B10</f>
+        <v>Benešov</v>
+      </c>
+      <c r="B3" s="18">
+        <f>DATA!C10</f>
+        <v>1732</v>
+      </c>
+      <c r="C3" s="18">
+        <f>DATA!G10</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="18" t="str">
+        <f>DATA!B11</f>
+        <v>Beroun</v>
+      </c>
+      <c r="B4" s="18">
+        <f>DATA!C11</f>
+        <v>1707</v>
+      </c>
+      <c r="C4" s="18">
+        <f>DATA!G11</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="18" t="str">
+        <f>DATA!B12</f>
+        <v>Kladno</v>
+      </c>
+      <c r="B5" s="18">
+        <f>DATA!C12</f>
+        <v>3300</v>
+      </c>
+      <c r="C5" s="18">
+        <f>DATA!G12</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="str">
+        <f>DATA!B13</f>
+        <v>Kolín</v>
+      </c>
+      <c r="B6" s="18">
+        <f>DATA!C13</f>
+        <v>2047</v>
+      </c>
+      <c r="C6" s="18">
+        <f>DATA!G13</f>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="18" t="str">
+        <f>DATA!B14</f>
+        <v>Kutná Hora</v>
+      </c>
+      <c r="B7" s="18">
+        <f>DATA!C14</f>
+        <v>1000</v>
+      </c>
+      <c r="C7" s="18">
+        <f>DATA!G14</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="18" t="str">
+        <f>DATA!B15</f>
+        <v>Mělník</v>
+      </c>
+      <c r="B8" s="18">
+        <f>DATA!C15</f>
+        <v>1861</v>
+      </c>
+      <c r="C8" s="18">
+        <f>DATA!G15</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="str">
+        <f>DATA!B16</f>
+        <v>Mladá Boleslav</v>
+      </c>
+      <c r="B9" s="18">
+        <f>DATA!C16</f>
+        <v>2531</v>
+      </c>
+      <c r="C9" s="18">
+        <f>DATA!G16</f>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="str">
+        <f>DATA!B17</f>
+        <v>Nymburk</v>
+      </c>
+      <c r="B10" s="18">
+        <f>DATA!C17</f>
+        <v>1588</v>
+      </c>
+      <c r="C10" s="18">
+        <f>DATA!G17</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="str">
+        <f>DATA!B18</f>
+        <v>Praha-východ</v>
+      </c>
+      <c r="B11" s="18">
+        <f>DATA!C18</f>
+        <v>3638</v>
+      </c>
+      <c r="C11" s="18">
+        <f>DATA!G18</f>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="18" t="str">
+        <f>DATA!B19</f>
+        <v>Praha-západ</v>
+      </c>
+      <c r="B12" s="18">
+        <f>DATA!C19</f>
+        <v>2851</v>
+      </c>
+      <c r="C12" s="18">
+        <f>DATA!G19</f>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="str">
+        <f>DATA!B20</f>
+        <v>Příbram</v>
+      </c>
+      <c r="B13" s="18">
+        <f>DATA!C20</f>
+        <v>2247</v>
+      </c>
+      <c r="C13" s="18">
+        <f>DATA!G20</f>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="str">
+        <f>DATA!B21</f>
+        <v>Rakovník</v>
+      </c>
+      <c r="B14" s="18">
+        <f>DATA!C21</f>
+        <v>940</v>
+      </c>
+      <c r="C14" s="18">
+        <f>DATA!G21</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="18" t="str">
+        <f>DATA!B23</f>
+        <v>České Budějovice</v>
+      </c>
+      <c r="B15" s="18">
+        <f>DATA!C23</f>
+        <v>5008</v>
+      </c>
+      <c r="C15" s="18">
+        <f>DATA!G23</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="18" t="str">
+        <f>DATA!B24</f>
+        <v>Český Krumlov</v>
+      </c>
+      <c r="B16" s="18">
+        <f>DATA!C24</f>
+        <v>1375</v>
+      </c>
+      <c r="C16" s="18">
+        <f>DATA!G24</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="18" t="str">
+        <f>DATA!B25</f>
+        <v>Jindřichův Hradec</v>
+      </c>
+      <c r="B17" s="18">
+        <f>DATA!C25</f>
+        <v>1372</v>
+      </c>
+      <c r="C17" s="18">
+        <f>DATA!G25</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="18" t="str">
+        <f>DATA!B26</f>
+        <v>Písek</v>
+      </c>
+      <c r="B18" s="18">
+        <f>DATA!C26</f>
+        <v>1323</v>
+      </c>
+      <c r="C18" s="18">
+        <f>DATA!G26</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="18" t="str">
+        <f>DATA!B27</f>
+        <v>Prachatice</v>
+      </c>
+      <c r="B19" s="18">
+        <f>DATA!C27</f>
+        <v>888</v>
+      </c>
+      <c r="C19" s="18">
+        <f>DATA!G27</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="18" t="str">
+        <f>DATA!B28</f>
+        <v>Strakonice</v>
+      </c>
+      <c r="B20" s="18">
+        <f>DATA!C28</f>
+        <v>1252</v>
+      </c>
+      <c r="C20" s="18">
+        <f>DATA!G28</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="18" t="str">
+        <f>DATA!B29</f>
+        <v>Tábor</v>
+      </c>
+      <c r="B21" s="18">
+        <f>DATA!C29</f>
+        <v>1377</v>
+      </c>
+      <c r="C21" s="18">
+        <f>DATA!G29</f>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="18" t="str">
+        <f>DATA!B31</f>
+        <v>Domažlice</v>
+      </c>
+      <c r="B22" s="18">
+        <f>DATA!C31</f>
+        <v>940</v>
+      </c>
+      <c r="C22" s="18">
+        <f>DATA!G31</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="18" t="str">
+        <f>DATA!B32</f>
+        <v>Klatovy</v>
+      </c>
+      <c r="B23" s="18">
+        <f>DATA!C32</f>
+        <v>1145</v>
+      </c>
+      <c r="C23" s="18">
+        <f>DATA!G32</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="18" t="str">
+        <f>DATA!B33</f>
+        <v>Plzeň-město</v>
+      </c>
+      <c r="B24" s="18">
+        <f>DATA!C33</f>
+        <v>5244</v>
+      </c>
+      <c r="C24" s="18">
+        <f>DATA!G33</f>
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="str">
+        <f>DATA!B34</f>
+        <v>Plzeň-jih</v>
+      </c>
+      <c r="B25" s="18">
+        <f>DATA!C34</f>
+        <v>638</v>
+      </c>
+      <c r="C25" s="18">
+        <f>DATA!G34</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="str">
+        <f>DATA!B35</f>
+        <v>Plzeň-sever</v>
+      </c>
+      <c r="B26" s="18">
+        <f>DATA!C35</f>
+        <v>915</v>
+      </c>
+      <c r="C26" s="18">
+        <f>DATA!G35</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="18" t="str">
+        <f>DATA!B36</f>
+        <v>Rokycany</v>
+      </c>
+      <c r="B27" s="18">
+        <f>DATA!C36</f>
+        <v>664</v>
+      </c>
+      <c r="C27" s="18">
+        <f>DATA!G36</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="18" t="str">
+        <f>DATA!B37</f>
+        <v>Tachov</v>
+      </c>
+      <c r="B28" s="18">
+        <f>DATA!C37</f>
+        <v>966</v>
+      </c>
+      <c r="C28" s="18">
+        <f>DATA!G37</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="18" t="str">
+        <f>DATA!B39</f>
+        <v>Cheb</v>
+      </c>
+      <c r="B29" s="18">
+        <f>DATA!C39</f>
+        <v>1769</v>
+      </c>
+      <c r="C29" s="18">
+        <f>DATA!G39</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="18" t="str">
+        <f>DATA!B40</f>
+        <v>Karlovy Vary</v>
+      </c>
+      <c r="B30" s="18">
+        <f>DATA!C40</f>
+        <v>2478</v>
+      </c>
+      <c r="C30" s="18">
+        <f>DATA!G40</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="18" t="str">
+        <f>DATA!B41</f>
+        <v>Sokolov</v>
+      </c>
+      <c r="B31" s="18">
+        <f>DATA!C41</f>
+        <v>1490</v>
+      </c>
+      <c r="C31" s="18">
+        <f>DATA!G41</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="18" t="str">
+        <f>DATA!B43</f>
+        <v>Děčín</v>
+      </c>
+      <c r="B32" s="18">
+        <f>DATA!C43</f>
+        <v>3316</v>
+      </c>
+      <c r="C32" s="18">
+        <f>DATA!G43</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="str">
+        <f>DATA!B44</f>
+        <v>Chomutov</v>
+      </c>
+      <c r="B33" s="18">
+        <f>DATA!C44</f>
+        <v>3083</v>
+      </c>
+      <c r="C33" s="18">
+        <f>DATA!G44</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="18" t="str">
+        <f>DATA!B45</f>
+        <v>Litoměřice</v>
+      </c>
+      <c r="B34" s="18">
+        <f>DATA!C45</f>
+        <v>2455</v>
+      </c>
+      <c r="C34" s="18">
+        <f>DATA!G45</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="str">
+        <f>DATA!B46</f>
+        <v>Louny</v>
+      </c>
+      <c r="B35" s="18">
+        <f>DATA!C46</f>
+        <v>1588</v>
+      </c>
+      <c r="C35" s="18">
+        <f>DATA!G46</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="str">
+        <f>DATA!B47</f>
+        <v>Most</v>
+      </c>
+      <c r="B36" s="18">
+        <f>DATA!C47</f>
+        <v>3575</v>
+      </c>
+      <c r="C36" s="18">
+        <f>DATA!G47</f>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="str">
+        <f>DATA!B48</f>
+        <v>Teplice</v>
+      </c>
+      <c r="B37" s="18">
+        <f>DATA!C48</f>
+        <v>3450</v>
+      </c>
+      <c r="C37" s="18">
+        <f>DATA!G48</f>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="str">
+        <f>DATA!B49</f>
+        <v>Ústí nad Labem</v>
+      </c>
+      <c r="B38" s="18">
+        <f>DATA!C49</f>
+        <v>3594</v>
+      </c>
+      <c r="C38" s="18">
+        <f>DATA!G49</f>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="18" t="str">
+        <f>DATA!B51</f>
+        <v>Česká Lípa</v>
+      </c>
+      <c r="B39" s="18">
+        <f>DATA!C51</f>
+        <v>2988</v>
+      </c>
+      <c r="C39" s="18">
+        <f>DATA!G51</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="18" t="str">
+        <f>DATA!B52</f>
+        <v>Jablonec nad Nisou</v>
+      </c>
+      <c r="B40" s="18">
+        <f>DATA!C52</f>
+        <v>1951</v>
+      </c>
+      <c r="C40" s="18">
+        <f>DATA!G52</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="18" t="str">
+        <f>DATA!B53</f>
+        <v>Liberec</v>
+      </c>
+      <c r="B41" s="18">
+        <f>DATA!C53</f>
+        <v>5045</v>
+      </c>
+      <c r="C41" s="18">
+        <f>DATA!G53</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="str">
+        <f>DATA!B54</f>
+        <v>Semily</v>
+      </c>
+      <c r="B42" s="18">
+        <f>DATA!C54</f>
+        <v>1170</v>
+      </c>
+      <c r="C42" s="18">
+        <f>DATA!G54</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="18" t="str">
+        <f>DATA!B56</f>
+        <v>Hradec Králové</v>
+      </c>
+      <c r="B43" s="18">
+        <f>DATA!C56</f>
+        <v>2555</v>
+      </c>
+      <c r="C43" s="18">
+        <f>DATA!G56</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="18" t="str">
+        <f>DATA!B57</f>
+        <v>Jičín</v>
+      </c>
+      <c r="B44" s="18">
+        <f>DATA!C57</f>
+        <v>1210</v>
+      </c>
+      <c r="C44" s="18">
+        <f>DATA!G57</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="18" t="str">
+        <f>DATA!B58</f>
+        <v>Náchod</v>
+      </c>
+      <c r="B45" s="18">
+        <f>DATA!C58</f>
+        <v>1830</v>
+      </c>
+      <c r="C45" s="18">
+        <f>DATA!G58</f>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="18" t="str">
+        <f>DATA!B59</f>
+        <v>Rychnov nad Kněžnou</v>
+      </c>
+      <c r="B46" s="18">
+        <f>DATA!C59</f>
+        <v>965</v>
+      </c>
+      <c r="C46" s="18">
+        <f>DATA!G59</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="18" t="str">
+        <f>DATA!B60</f>
+        <v>Trutnov</v>
+      </c>
+      <c r="B47" s="18">
+        <f>DATA!C60</f>
+        <v>2015</v>
+      </c>
+      <c r="C47" s="18">
+        <f>DATA!G60</f>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="18" t="str">
+        <f>DATA!B62</f>
+        <v>Chrudim</v>
+      </c>
+      <c r="B48" s="18">
+        <f>DATA!C62</f>
+        <v>1171</v>
+      </c>
+      <c r="C48" s="18">
+        <f>DATA!G62</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="18" t="str">
+        <f>DATA!B63</f>
+        <v>Pardubice</v>
+      </c>
+      <c r="B49" s="18">
+        <f>DATA!C63</f>
+        <v>2987</v>
+      </c>
+      <c r="C49" s="18">
+        <f>DATA!G63</f>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="18" t="str">
+        <f>DATA!B64</f>
+        <v>Svitavy</v>
+      </c>
+      <c r="B50" s="18">
+        <f>DATA!C64</f>
+        <v>1223</v>
+      </c>
+      <c r="C50" s="18">
+        <f>DATA!G64</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="18" t="str">
+        <f>DATA!B65</f>
+        <v>Ústí nad Orlicí</v>
+      </c>
+      <c r="B51" s="18">
+        <f>DATA!C65</f>
+        <v>1431</v>
+      </c>
+      <c r="C51" s="18">
+        <f>DATA!G65</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="18" t="str">
+        <f>DATA!B67</f>
+        <v>Havlíčkův Brod</v>
+      </c>
+      <c r="B52" s="18">
+        <f>DATA!C67</f>
+        <v>1269</v>
+      </c>
+      <c r="C52" s="18">
+        <f>DATA!G67</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="18" t="str">
+        <f>DATA!B68</f>
+        <v>Jihlava</v>
+      </c>
+      <c r="B53" s="18">
+        <f>DATA!C68</f>
+        <v>1910</v>
+      </c>
+      <c r="C53" s="18">
+        <f>DATA!G68</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="18" t="str">
+        <f>DATA!B69</f>
+        <v>Pelhřimov</v>
+      </c>
+      <c r="B54" s="18">
+        <f>DATA!C69</f>
+        <v>1007</v>
+      </c>
+      <c r="C54" s="18">
+        <f>DATA!G69</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="18" t="str">
+        <f>DATA!B70</f>
+        <v>Třebíč</v>
+      </c>
+      <c r="B55" s="18">
+        <f>DATA!C70</f>
+        <v>1437</v>
+      </c>
+      <c r="C55" s="18">
+        <f>DATA!G70</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="18" t="str">
+        <f>DATA!B71</f>
+        <v>Žďár nad Sázavou</v>
+      </c>
+      <c r="B56" s="18">
+        <f>DATA!C71</f>
+        <v>1257</v>
+      </c>
+      <c r="C56" s="18">
+        <f>DATA!G71</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="18" t="str">
+        <f>DATA!B73</f>
+        <v>Blansko</v>
+      </c>
+      <c r="B57" s="18">
+        <f>DATA!C73</f>
+        <v>1375</v>
+      </c>
+      <c r="C57" s="18">
+        <f>DATA!G73</f>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="18" t="str">
+        <f>DATA!B74</f>
+        <v>Brno-město</v>
+      </c>
+      <c r="B58" s="18">
+        <f>DATA!C74</f>
+        <v>12918</v>
+      </c>
+      <c r="C58" s="18">
+        <f>DATA!G74</f>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="18" t="str">
+        <f>DATA!B75</f>
+        <v>Brno-venkov</v>
+      </c>
+      <c r="B59" s="18">
+        <f>DATA!C75</f>
+        <v>2916</v>
+      </c>
+      <c r="C59" s="18">
+        <f>DATA!G75</f>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="18" t="str">
+        <f>DATA!B76</f>
+        <v>Břeclav</v>
+      </c>
+      <c r="B60" s="18">
+        <f>DATA!C76</f>
+        <v>1757</v>
+      </c>
+      <c r="C60" s="18">
+        <f>DATA!G76</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="18" t="str">
+        <f>DATA!B77</f>
+        <v>Hodonín</v>
+      </c>
+      <c r="B61" s="18">
+        <f>DATA!C77</f>
+        <v>1765</v>
+      </c>
+      <c r="C61" s="18">
+        <f>DATA!G77</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="18" t="str">
+        <f>DATA!B78</f>
+        <v>Vyškov</v>
+      </c>
+      <c r="B62" s="18">
+        <f>DATA!C78</f>
+        <v>1119</v>
+      </c>
+      <c r="C62" s="18">
+        <f>DATA!G78</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="18" t="str">
+        <f>DATA!B79</f>
+        <v>Znojmo</v>
+      </c>
+      <c r="B63" s="18">
+        <f>DATA!C79</f>
+        <v>1978</v>
+      </c>
+      <c r="C63" s="18">
+        <f>DATA!G79</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="18" t="str">
+        <f>DATA!B81</f>
+        <v>Jeseník</v>
+      </c>
+      <c r="B64" s="18">
+        <f>DATA!C81</f>
+        <v>787</v>
+      </c>
+      <c r="C64" s="18">
+        <f>DATA!G81</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="18" t="str">
+        <f>DATA!B82</f>
+        <v>Olomouc</v>
+      </c>
+      <c r="B65" s="18">
+        <f>DATA!C82</f>
+        <v>5265</v>
+      </c>
+      <c r="C65" s="18">
+        <f>DATA!G82</f>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="18" t="str">
+        <f>DATA!B83</f>
+        <v>Prostějov</v>
+      </c>
+      <c r="B66" s="18">
+        <f>DATA!C83</f>
+        <v>2059</v>
+      </c>
+      <c r="C66" s="18">
+        <f>DATA!G83</f>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="18" t="str">
+        <f>DATA!B84</f>
+        <v>Přerov</v>
+      </c>
+      <c r="B67" s="18">
+        <f>DATA!C84</f>
+        <v>2432</v>
+      </c>
+      <c r="C67" s="18">
+        <f>DATA!G84</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="18" t="str">
+        <f>DATA!B85</f>
+        <v>Šumperk</v>
+      </c>
+      <c r="B68" s="18">
+        <f>DATA!C85</f>
+        <v>2066</v>
+      </c>
+      <c r="C68" s="18">
+        <f>DATA!G85</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="18" t="str">
+        <f>DATA!B87</f>
+        <v>Kroměříž</v>
+      </c>
+      <c r="B69" s="18">
+        <f>DATA!C87</f>
+        <v>1465</v>
+      </c>
+      <c r="C69" s="18">
+        <f>DATA!G87</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="18" t="str">
+        <f>DATA!B88</f>
+        <v>Uherské Hradiště</v>
+      </c>
+      <c r="B70" s="18">
+        <f>DATA!C88</f>
+        <v>1790</v>
+      </c>
+      <c r="C70" s="18">
+        <f>DATA!G88</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="18" t="str">
+        <f>DATA!B89</f>
+        <v>Vsetín</v>
+      </c>
+      <c r="B71" s="18">
+        <f>DATA!C89</f>
+        <v>2135</v>
+      </c>
+      <c r="C71" s="18">
+        <f>DATA!G89</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="18" t="str">
+        <f>DATA!B90</f>
+        <v>Zlín</v>
+      </c>
+      <c r="B72" s="18">
+        <f>DATA!C90</f>
+        <v>2574</v>
+      </c>
+      <c r="C72" s="18">
+        <f>DATA!G90</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="18" t="str">
+        <f>DATA!B92</f>
+        <v>Bruntál</v>
+      </c>
+      <c r="B73" s="18">
+        <f>DATA!C92</f>
+        <v>1858</v>
+      </c>
+      <c r="C73" s="18">
+        <f>DATA!G92</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="18" t="str">
+        <f>DATA!B93</f>
+        <v>Frýdek-Místek</v>
+      </c>
+      <c r="B74" s="18">
+        <f>DATA!C93</f>
+        <v>3812</v>
+      </c>
+      <c r="C74" s="18">
+        <f>DATA!G93</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="18" t="str">
+        <f>DATA!B94</f>
+        <v>Karviná</v>
+      </c>
+      <c r="B75" s="18">
+        <f>DATA!C94</f>
+        <v>6331</v>
+      </c>
+      <c r="C75" s="18">
+        <f>DATA!G94</f>
+        <v>272</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="18" t="str">
+        <f>DATA!B95</f>
+        <v>Nový Jičín</v>
+      </c>
+      <c r="B76" s="18">
+        <f>DATA!C95</f>
+        <v>2657</v>
+      </c>
+      <c r="C76" s="18">
+        <f>DATA!G95</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="18" t="str">
+        <f>DATA!B96</f>
+        <v>Opava</v>
+      </c>
+      <c r="B77" s="18">
+        <f>DATA!C96</f>
+        <v>2957</v>
+      </c>
+      <c r="C77" s="18">
+        <f>DATA!G96</f>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="18" t="str">
+        <f>DATA!B97</f>
+        <v>Ostrava-město</v>
+      </c>
+      <c r="B78" s="18">
+        <f>DATA!C97</f>
+        <v>12749</v>
+      </c>
+      <c r="C78" s="18">
+        <f>DATA!G97</f>
+        <v>252</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="18"/>
+      <c r="B79" s="18"/>
+      <c r="C79" s="18"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="18"/>
+      <c r="B80" s="18"/>
+      <c r="C80" s="18"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="18"/>
+      <c r="B81" s="18"/>
+      <c r="C81" s="18"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="18"/>
+      <c r="B82" s="18"/>
+      <c r="C82" s="18"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="18"/>
+      <c r="B83" s="18"/>
+      <c r="C83" s="18"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="18"/>
+      <c r="B84" s="18"/>
+      <c r="C84" s="18"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="18"/>
+      <c r="B85" s="18"/>
+      <c r="C85" s="18"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="18"/>
+      <c r="B86" s="18"/>
+      <c r="C86" s="18"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="18"/>
+      <c r="B87" s="18"/>
+      <c r="C87" s="18"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="18"/>
+      <c r="B88" s="18"/>
+      <c r="C88" s="18"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="18"/>
+      <c r="B89" s="18"/>
+      <c r="C89" s="18"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="18"/>
+      <c r="B90" s="18"/>
+      <c r="C90" s="18"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="18"/>
+      <c r="B91" s="18"/>
+      <c r="C91" s="18"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="18"/>
+      <c r="B92" s="18"/>
+      <c r="C92" s="18"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="18"/>
+      <c r="B93" s="18"/>
+      <c r="C93" s="18"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="18"/>
+      <c r="B94" s="18"/>
+      <c r="C94" s="18"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="18"/>
+      <c r="B95" s="18"/>
+      <c r="C95" s="18"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="18"/>
+      <c r="B96" s="18"/>
+      <c r="C96" s="18"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="18"/>
+      <c r="B97" s="18"/>
+      <c r="C97" s="18"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="18"/>
+      <c r="B98" s="18"/>
+      <c r="C98" s="18"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="18"/>
+      <c r="B99" s="18"/>
+      <c r="C99" s="18"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="18"/>
+      <c r="B100" s="18"/>
+      <c r="C100" s="18"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="18"/>
+      <c r="B101" s="18"/>
+      <c r="C101" s="18"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="18"/>
+      <c r="B102" s="18"/>
+      <c r="C102" s="18"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="18"/>
+      <c r="B103" s="18"/>
+      <c r="C103" s="18"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="18"/>
+      <c r="B104" s="18"/>
+      <c r="C104" s="18"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="18"/>
+      <c r="B105" s="18"/>
+      <c r="C105" s="18"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="18"/>
+      <c r="B106" s="18"/>
+      <c r="C106" s="18"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="18"/>
+      <c r="B107" s="18"/>
+      <c r="C107" s="18"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="18"/>
+      <c r="B108" s="18"/>
+      <c r="C108" s="18"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="18"/>
+      <c r="B109" s="18"/>
+      <c r="C109" s="18"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="18"/>
+      <c r="B110" s="18"/>
+      <c r="C110" s="18"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="18"/>
+      <c r="B111" s="18"/>
+      <c r="C111" s="18"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="18"/>
+      <c r="B112" s="18"/>
+      <c r="C112" s="18"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="18"/>
+      <c r="B113" s="18"/>
+      <c r="C113" s="18"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="18"/>
+      <c r="B114" s="18"/>
+      <c r="C114" s="18"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="18"/>
+      <c r="B115" s="18"/>
+      <c r="C115" s="18"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="18"/>
+      <c r="B116" s="18"/>
+      <c r="C116" s="18"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="18"/>
+      <c r="B117" s="18"/>
+      <c r="C117" s="18"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="18"/>
+      <c r="B118" s="18"/>
+      <c r="C118" s="18"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="18"/>
+      <c r="B119" s="18"/>
+      <c r="C119" s="18"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="18"/>
+      <c r="B120" s="18"/>
+      <c r="C120" s="18"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="18"/>
+      <c r="B121" s="18"/>
+      <c r="C121" s="18"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="18"/>
+      <c r="B122" s="18"/>
+      <c r="C122" s="18"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="18"/>
+      <c r="B123" s="18"/>
+      <c r="C123" s="18"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="18"/>
+      <c r="B124" s="18"/>
+      <c r="C124" s="18"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="18"/>
+      <c r="B125" s="18"/>
+      <c r="C125" s="18"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="18"/>
+      <c r="B126" s="18"/>
+      <c r="C126" s="18"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="18"/>
+      <c r="B127" s="18"/>
+      <c r="C127" s="18"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="18"/>
+      <c r="B128" s="18"/>
+      <c r="C128" s="18"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="18"/>
+      <c r="B129" s="18"/>
+      <c r="C129" s="18"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="18"/>
+      <c r="B130" s="18"/>
+      <c r="C130" s="18"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="18"/>
+      <c r="B131" s="18"/>
+      <c r="C131" s="18"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="18"/>
+      <c r="B132" s="18"/>
+      <c r="C132" s="18"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="18"/>
+      <c r="B133" s="18"/>
+      <c r="C133" s="18"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="18"/>
+      <c r="B134" s="18"/>
+      <c r="C134" s="18"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="18"/>
+      <c r="B135" s="18"/>
+      <c r="C135" s="18"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="18"/>
+      <c r="B136" s="18"/>
+      <c r="C136" s="18"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="18"/>
+      <c r="B137" s="18"/>
+      <c r="C137" s="18"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="18"/>
+      <c r="B138" s="18"/>
+      <c r="C138" s="18"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="18"/>
+      <c r="B139" s="18"/>
+      <c r="C139" s="18"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="18"/>
+      <c r="B140" s="18"/>
+      <c r="C140" s="18"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="18"/>
+      <c r="B141" s="18"/>
+      <c r="C141" s="18"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="18"/>
+      <c r="B142" s="18"/>
+      <c r="C142" s="18"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="18"/>
+      <c r="B143" s="18"/>
+      <c r="C143" s="18"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="18"/>
+      <c r="B144" s="18"/>
+      <c r="C144" s="18"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="18"/>
+      <c r="B145" s="18"/>
+      <c r="C145" s="18"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="18"/>
+      <c r="B146" s="18"/>
+      <c r="C146" s="18"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="18"/>
+      <c r="B147" s="18"/>
+      <c r="C147" s="18"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="18"/>
+      <c r="B148" s="18"/>
+      <c r="C148" s="18"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="18"/>
+      <c r="B149" s="18"/>
+      <c r="C149" s="18"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" s="18"/>
+      <c r="B150" s="18"/>
+      <c r="C150" s="18"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="18"/>
+      <c r="B151" s="18"/>
+      <c r="C151" s="18"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" s="18"/>
+      <c r="B152" s="18"/>
+      <c r="C152" s="18"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" s="18"/>
+      <c r="B153" s="18"/>
+      <c r="C153" s="18"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" s="18"/>
+      <c r="B154" s="18"/>
+      <c r="C154" s="18"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" s="18"/>
+      <c r="B155" s="18"/>
+      <c r="C155" s="18"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" s="18"/>
+      <c r="B156" s="18"/>
+      <c r="C156" s="18"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="18"/>
+      <c r="B157" s="18"/>
+      <c r="C157" s="18"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" s="18"/>
+      <c r="B158" s="18"/>
+      <c r="C158" s="18"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" s="18"/>
+      <c r="B159" s="18"/>
+      <c r="C159" s="18"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" s="18"/>
+      <c r="B160" s="18"/>
+      <c r="C160" s="18"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" s="18"/>
+      <c r="B161" s="18"/>
+      <c r="C161" s="18"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" s="18"/>
+      <c r="B162" s="18"/>
+      <c r="C162" s="18"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" s="18"/>
+      <c r="B163" s="18"/>
+      <c r="C163" s="18"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" s="18"/>
+      <c r="B164" s="18"/>
+      <c r="C164" s="18"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" s="18"/>
+      <c r="B165" s="18"/>
+      <c r="C165" s="18"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" s="18"/>
+      <c r="B166" s="18"/>
+      <c r="C166" s="18"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="18"/>
+      <c r="B167" s="18"/>
+      <c r="C167" s="18"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" s="18"/>
+      <c r="B168" s="18"/>
+      <c r="C168" s="18"/>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" s="18"/>
+      <c r="B169" s="18"/>
+      <c r="C169" s="18"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="18"/>
+      <c r="B170" s="18"/>
+      <c r="C170" s="18"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="18"/>
+      <c r="B171" s="18"/>
+      <c r="C171" s="18"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A172" s="18"/>
+      <c r="B172" s="18"/>
+      <c r="C172" s="18"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A173" s="18"/>
+      <c r="B173" s="18"/>
+      <c r="C173" s="18"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A174" s="18"/>
+      <c r="B174" s="18"/>
+      <c r="C174" s="18"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A175" s="18"/>
+      <c r="B175" s="18"/>
+      <c r="C175" s="18"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A176" s="18"/>
+      <c r="B176" s="18"/>
+      <c r="C176" s="18"/>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A177" s="18"/>
+      <c r="B177" s="18"/>
+      <c r="C177" s="18"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A178" s="18"/>
+      <c r="B178" s="18"/>
+      <c r="C178" s="18"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A179" s="18"/>
+      <c r="B179" s="18"/>
+      <c r="C179" s="18"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A180" s="18"/>
+      <c r="B180" s="18"/>
+      <c r="C180" s="18"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A181" s="18"/>
+      <c r="B181" s="18"/>
+      <c r="C181" s="18"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A182" s="18"/>
+      <c r="B182" s="18"/>
+      <c r="C182" s="18"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A183" s="18"/>
+      <c r="B183" s="18"/>
+      <c r="C183" s="18"/>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A184" s="18"/>
+      <c r="B184" s="18"/>
+      <c r="C184" s="18"/>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A185" s="18"/>
+      <c r="B185" s="18"/>
+      <c r="C185" s="18"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A186" s="18"/>
+      <c r="B186" s="18"/>
+      <c r="C186" s="18"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A187" s="18"/>
+      <c r="B187" s="18"/>
+      <c r="C187" s="18"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A188" s="18"/>
+      <c r="B188" s="18"/>
+      <c r="C188" s="18"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A189" s="18"/>
+      <c r="B189" s="18"/>
+      <c r="C189" s="18"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A190" s="18"/>
+      <c r="B190" s="18"/>
+      <c r="C190" s="18"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A191" s="18"/>
+      <c r="B191" s="18"/>
+      <c r="C191" s="18"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A192" s="18"/>
+      <c r="B192" s="18"/>
+      <c r="C192" s="18"/>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A193" s="18"/>
+      <c r="B193" s="18"/>
+      <c r="C193" s="18"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A194" s="18"/>
+      <c r="B194" s="18"/>
+      <c r="C194" s="18"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A195" s="18"/>
+      <c r="B195" s="18"/>
+      <c r="C195" s="18"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A196" s="18"/>
+      <c r="B196" s="18"/>
+      <c r="C196" s="18"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A197" s="18"/>
+      <c r="B197" s="18"/>
+      <c r="C197" s="18"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A198" s="18"/>
+      <c r="B198" s="18"/>
+      <c r="C198" s="18"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A199" s="18"/>
+      <c r="B199" s="18"/>
+      <c r="C199" s="18"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A200" s="18"/>
+      <c r="B200" s="18"/>
+      <c r="C200" s="18"/>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A201" s="18"/>
+      <c r="B201" s="18"/>
+      <c r="C201" s="18"/>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A202" s="18"/>
+      <c r="B202" s="18"/>
+      <c r="C202" s="18"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A203" s="18"/>
+      <c r="B203" s="18"/>
+      <c r="C203" s="18"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A204" s="18"/>
+      <c r="B204" s="18"/>
+      <c r="C204" s="18"/>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A205" s="18"/>
+      <c r="B205" s="18"/>
+      <c r="C205" s="18"/>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A206" s="18"/>
+      <c r="B206" s="18"/>
+      <c r="C206" s="18"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A207" s="18"/>
+      <c r="B207" s="18"/>
+      <c r="C207" s="18"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A208" s="18"/>
+      <c r="B208" s="18"/>
+      <c r="C208" s="18"/>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A209" s="18"/>
+      <c r="B209" s="18"/>
+      <c r="C209" s="18"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A210" s="18"/>
+      <c r="B210" s="18"/>
+      <c r="C210" s="18"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A211" s="18"/>
+      <c r="B211" s="18"/>
+      <c r="C211" s="18"/>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A212" s="18"/>
+      <c r="B212" s="18"/>
+      <c r="C212" s="18"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A213" s="18"/>
+      <c r="B213" s="18"/>
+      <c r="C213" s="18"/>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A214" s="18"/>
+      <c r="B214" s="18"/>
+      <c r="C214" s="18"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A215" s="18"/>
+      <c r="B215" s="18"/>
+      <c r="C215" s="18"/>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A216" s="18"/>
+      <c r="B216" s="18"/>
+      <c r="C216" s="18"/>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A217" s="18"/>
+      <c r="B217" s="18"/>
+      <c r="C217" s="18"/>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A218" s="18"/>
+      <c r="B218" s="18"/>
+      <c r="C218" s="18"/>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A219" s="18"/>
+      <c r="B219" s="18"/>
+      <c r="C219" s="18"/>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A220" s="18"/>
+      <c r="B220" s="18"/>
+      <c r="C220" s="18"/>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A221" s="18"/>
+      <c r="B221" s="18"/>
+      <c r="C221" s="18"/>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A222" s="18"/>
+      <c r="B222" s="18"/>
+      <c r="C222" s="18"/>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A223" s="18"/>
+      <c r="B223" s="18"/>
+      <c r="C223" s="18"/>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A224" s="18"/>
+      <c r="B224" s="18"/>
+      <c r="C224" s="18"/>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A225" s="18"/>
+      <c r="B225" s="18"/>
+      <c r="C225" s="18"/>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A226" s="18"/>
+      <c r="B226" s="18"/>
+      <c r="C226" s="18"/>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A227" s="18"/>
+      <c r="B227" s="18"/>
+      <c r="C227" s="18"/>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A228" s="18"/>
+      <c r="B228" s="18"/>
+      <c r="C228" s="18"/>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A229" s="18"/>
+      <c r="B229" s="18"/>
+      <c r="C229" s="18"/>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A230" s="18"/>
+      <c r="B230" s="18"/>
+      <c r="C230" s="18"/>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A231" s="18"/>
+      <c r="B231" s="18"/>
+      <c r="C231" s="18"/>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" s="18"/>
+      <c r="B232" s="18"/>
+      <c r="C232" s="18"/>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" s="18"/>
+      <c r="B233" s="18"/>
+      <c r="C233" s="18"/>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" s="18"/>
+      <c r="B234" s="18"/>
+      <c r="C234" s="18"/>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" s="18"/>
+      <c r="B235" s="18"/>
+      <c r="C235" s="18"/>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" s="18"/>
+      <c r="B236" s="18"/>
+      <c r="C236" s="18"/>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" s="18"/>
+      <c r="B237" s="18"/>
+      <c r="C237" s="18"/>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" s="18"/>
+      <c r="B238" s="18"/>
+      <c r="C238" s="18"/>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" s="18"/>
+      <c r="B239" s="18"/>
+      <c r="C239" s="18"/>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" s="18"/>
+      <c r="B240" s="18"/>
+      <c r="C240" s="18"/>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" s="18"/>
+      <c r="B241" s="18"/>
+      <c r="C241" s="18"/>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A242" s="18"/>
+      <c r="B242" s="18"/>
+      <c r="C242" s="18"/>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A243" s="18"/>
+      <c r="B243" s="18"/>
+      <c r="C243" s="18"/>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A244" s="18"/>
+      <c r="B244" s="18"/>
+      <c r="C244" s="18"/>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A245" s="18"/>
+      <c r="B245" s="18"/>
+      <c r="C245" s="18"/>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A246" s="18"/>
+      <c r="B246" s="18"/>
+      <c r="C246" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3763,11 +5719,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3838,7 +5796,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F118"/>
   <sheetViews>

</xml_diff>